<commit_message>
working on page before confirm
</commit_message>
<xml_diff>
--- a/Week6/Assignment/TestAutomation/src/test/resources/MercuryData.xlsx
+++ b/Week6/Assignment/TestAutomation/src/test/resources/MercuryData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynda\Documents\Work\RevatureQTraining\180121_SDET\Week6\Assignment\TestAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0166871-16F0-4A33-AB75-D4871E8E6A5C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE1AD20-CDE3-4F69-8456-31EB20AD8E64}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="FlightFinder" sheetId="2" r:id="rId2"/>
+    <sheet name="Flight" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -40,12 +41,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{8BB43DB4-DAE1-49E3-AD22-46F9A8035D96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>value between 0 - 9</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -96,6 +111,12 @@
   </si>
   <si>
     <t>airline</t>
+  </si>
+  <si>
+    <t>depart</t>
+  </si>
+  <si>
+    <t>return</t>
   </si>
 </sst>
 </file>
@@ -522,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8859F885-66BA-4ADA-9D1C-379C2BCA442C}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -597,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>11</v>
@@ -691,4 +712,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB58492-EA9D-4962-8FDA-75355A44DF9C}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>